<commit_message>
Removed Test Case Inter-Dependency
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2425-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-DATE-VAR-INST-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/2425-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-DATE-VAR-INST-Newcreateloan1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>validate</t>
   </si>
   <si>
-    <t>2425-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-DATE-VAR-INST</t>
-  </si>
-  <si>
     <t>waittopageload</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>waittopageload1</t>
+  </si>
+  <si>
+    <t>2425-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-DATE-VAR-INST-1st</t>
   </si>
 </sst>
 </file>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +666,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>54</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="18">
         <v>2000</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="17">
         <v>42050</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>55</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="18">
         <v>2000</v>

</xml_diff>